<commit_message>
Update edited session - 2025-09-23T10:21:29.425Z - Cache Bust ID: 1758622889425i9ns8mrrv
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Dermatology_scanner1758615986194_7f7be7873d7924a649d56275a209274e4042011363951c41c7bc014e23c74d06.xlsx
+++ b/log_history/Y4_B2526_Dermatology_scanner1758615986194_7f7be7873d7924a649d56275a209274e4042011363951c41c7bc014e23c74d06.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>888096</v>
+        <v>222064</v>
       </c>
       <c r="B33" t="str">
         <v>Dermatology</v>
@@ -1053,7 +1053,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>11:34:52</v>
+        <v>11:35:11</v>
       </c>
       <c r="E33" t="str">
         <v>Manual</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>222064</v>
+        <v>221847</v>
       </c>
       <c r="B34" t="str">
         <v>Dermatology</v>
@@ -1073,7 +1073,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>11:35:11</v>
+        <v>11:35:22</v>
       </c>
       <c r="E34" t="str">
         <v>Manual</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>221847</v>
+        <v>222075</v>
       </c>
       <c r="B35" t="str">
         <v>Dermatology</v>
@@ -1093,7 +1093,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>11:35:22</v>
+        <v>11:35:32</v>
       </c>
       <c r="E35" t="str">
         <v>Manual</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>222075</v>
+        <v>221891</v>
       </c>
       <c r="B36" t="str">
         <v>Dermatology</v>
@@ -1113,7 +1113,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>11:35:32</v>
+        <v>11:35:45</v>
       </c>
       <c r="E36" t="str">
         <v>Manual</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>221891</v>
+        <v>222102</v>
       </c>
       <c r="B37" t="str">
         <v>Dermatology</v>
@@ -1133,7 +1133,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>11:35:45</v>
+        <v>11:35:49</v>
       </c>
       <c r="E37" t="str">
         <v>Manual</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>222102</v>
+        <v>221885</v>
       </c>
       <c r="B38" t="str">
         <v>Dermatology</v>
@@ -1153,7 +1153,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>11:35:49</v>
+        <v>11:35:53</v>
       </c>
       <c r="E38" t="str">
         <v>Manual</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>221885</v>
+        <v>221872</v>
       </c>
       <c r="B39" t="str">
         <v>Dermatology</v>
@@ -1173,7 +1173,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>11:35:53</v>
+        <v>11:35:57</v>
       </c>
       <c r="E39" t="str">
         <v>Manual</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>221872</v>
+        <v>221813</v>
       </c>
       <c r="B40" t="str">
         <v>Dermatology</v>
@@ -1193,7 +1193,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>11:35:57</v>
+        <v>11:36:13</v>
       </c>
       <c r="E40" t="str">
         <v>Manual</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>221813</v>
+        <v>221859</v>
       </c>
       <c r="B41" t="str">
         <v>Dermatology</v>
@@ -1213,7 +1213,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>11:36:13</v>
+        <v>11:36:17</v>
       </c>
       <c r="E41" t="str">
         <v>Manual</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>221859</v>
+        <v>221974</v>
       </c>
       <c r="B42" t="str">
         <v>Dermatology</v>
@@ -1233,7 +1233,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>11:36:17</v>
+        <v>11:36:26</v>
       </c>
       <c r="E42" t="str">
         <v>Manual</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>221974</v>
+        <v>222111</v>
       </c>
       <c r="B43" t="str">
         <v>Dermatology</v>
@@ -1253,7 +1253,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>11:36:26</v>
+        <v>11:36:30</v>
       </c>
       <c r="E43" t="str">
         <v>Manual</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>222111</v>
+        <v>221877</v>
       </c>
       <c r="B44" t="str">
         <v>Dermatology</v>
@@ -1273,7 +1273,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>11:36:30</v>
+        <v>11:36:37</v>
       </c>
       <c r="E44" t="str">
         <v>Manual</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>221877</v>
+        <v>222050</v>
       </c>
       <c r="B45" t="str">
         <v>Dermatology</v>
@@ -1293,7 +1293,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>11:36:37</v>
+        <v>11:36:40</v>
       </c>
       <c r="E45" t="str">
         <v>Manual</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>222050</v>
+        <v>221773</v>
       </c>
       <c r="B46" t="str">
         <v>Dermatology</v>
@@ -1313,7 +1313,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>11:36:40</v>
+        <v>11:36:45</v>
       </c>
       <c r="E46" t="str">
         <v>Manual</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>221773</v>
+        <v>221832</v>
       </c>
       <c r="B47" t="str">
         <v>Dermatology</v>
@@ -1333,7 +1333,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>11:36:45</v>
+        <v>11:36:48</v>
       </c>
       <c r="E47" t="str">
         <v>Manual</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>221832</v>
+        <v>222098</v>
       </c>
       <c r="B48" t="str">
         <v>Dermatology</v>
@@ -1353,7 +1353,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>11:36:48</v>
+        <v>11:36:54</v>
       </c>
       <c r="E48" t="str">
         <v>Manual</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>222098</v>
+        <v>221914</v>
       </c>
       <c r="B49" t="str">
         <v>Dermatology</v>
@@ -1373,7 +1373,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>11:36:54</v>
+        <v>11:36:58</v>
       </c>
       <c r="E49" t="str">
         <v>Manual</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>221914</v>
+        <v>221805</v>
       </c>
       <c r="B50" t="str">
         <v>Dermatology</v>
@@ -1393,7 +1393,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>11:36:58</v>
+        <v>11:37:05</v>
       </c>
       <c r="E50" t="str">
         <v>Manual</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>221805</v>
+        <v>221880</v>
       </c>
       <c r="B51" t="str">
         <v>Dermatology</v>
@@ -1413,7 +1413,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>11:37:05</v>
+        <v>11:37:13</v>
       </c>
       <c r="E51" t="str">
         <v>Manual</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>221880</v>
+        <v>222080</v>
       </c>
       <c r="B52" t="str">
         <v>Dermatology</v>
@@ -1433,7 +1433,7 @@
         <v>23/09/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>11:37:13</v>
+        <v>11:37:24</v>
       </c>
       <c r="E52" t="str">
         <v>Manual</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>222080</v>
+        <v>222094</v>
       </c>
       <c r="B53" t="str">
         <v>Dermatology</v>
@@ -1453,38 +1453,18 @@
         <v>23/09/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>11:37:24</v>
+        <v>11:37:35</v>
       </c>
       <c r="E53" t="str">
         <v>Manual</v>
       </c>
       <c r="F53" t="str">
-        <v>Mai.elsebaie@gmail.com</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="str">
-        <v>222094</v>
-      </c>
-      <c r="B54" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C54" t="str">
-        <v>23/09/2025</v>
-      </c>
-      <c r="D54" t="str">
-        <v>11:37:35</v>
-      </c>
-      <c r="E54" t="str">
-        <v>Manual</v>
-      </c>
-      <c r="F54" t="str">
         <v>Mai.elsebaie@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F54"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F53"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>